<commit_message>
Added multiple PVD1s on the same bus.
</commit_message>
<xml_diff>
--- a/andes/cases/ieee14/ieee14_pvd1.xlsx
+++ b/andes/cases/ieee14/ieee14_pvd1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcui7/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55528C2-D3F1-054C-8961-8AEA5BAE3B16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A45220-584E-0747-9881-4C2E495B8252}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="24280" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28840" yWindow="5460" windowWidth="24280" windowHeight="16160" firstSheet="1" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Toggler" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="201">
   <si>
     <t>idx</t>
   </si>
@@ -603,6 +603,39 @@
   </si>
   <si>
     <t>Toggler_2</t>
+  </si>
+  <si>
+    <t>gammap</t>
+  </si>
+  <si>
+    <t>gammaq</t>
+  </si>
+  <si>
+    <t>PVD1_2</t>
+  </si>
+  <si>
+    <t>PVD1_3</t>
+  </si>
+  <si>
+    <t>PVD1_4</t>
+  </si>
+  <si>
+    <t>PVD1_5</t>
+  </si>
+  <si>
+    <t>PVD1_6</t>
+  </si>
+  <si>
+    <t>PVD1_7</t>
+  </si>
+  <si>
+    <t>PVD1_8</t>
+  </si>
+  <si>
+    <t>PVD1_9</t>
+  </si>
+  <si>
+    <t>PVD1_10</t>
   </si>
 </sst>
 </file>
@@ -634,7 +667,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -657,13 +690,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1006,7 +1053,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
@@ -1917,16 +1964,16 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:AF2"/>
+  <dimension ref="A1:AH11"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
+      <selection pane="bottomLeft" activeCell="AH2" sqref="AH2:AH11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -2023,8 +2070,14 @@
       <c r="AF1" s="1" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG1" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2056,7 +2109,7 @@
         <v>0.2</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2">
         <v>0.33</v>
@@ -2117,6 +2170,921 @@
       </c>
       <c r="AF2">
         <v>0.02</v>
+      </c>
+      <c r="AG2">
+        <v>0.1</v>
+      </c>
+      <c r="AH2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>192</v>
+      </c>
+      <c r="E3">
+        <v>8</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>100</v>
+      </c>
+      <c r="H3">
+        <v>60</v>
+      </c>
+      <c r="I3" t="s">
+        <v>163</v>
+      </c>
+      <c r="J3">
+        <v>0.2</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0.33</v>
+      </c>
+      <c r="N3">
+        <v>-0.33</v>
+      </c>
+      <c r="O3">
+        <v>0.8</v>
+      </c>
+      <c r="P3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Q3">
+        <v>-1</v>
+      </c>
+      <c r="R3">
+        <v>-0.01</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>1.3</v>
+      </c>
+      <c r="U3">
+        <v>0.88</v>
+      </c>
+      <c r="V3">
+        <v>0.9</v>
+      </c>
+      <c r="W3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="X3">
+        <v>1.2</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>59.5</v>
+      </c>
+      <c r="AA3">
+        <v>59.7</v>
+      </c>
+      <c r="AB3">
+        <v>60.3</v>
+      </c>
+      <c r="AC3">
+        <v>60.5</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>0.02</v>
+      </c>
+      <c r="AF3">
+        <v>0.02</v>
+      </c>
+      <c r="AG3">
+        <v>0.1</v>
+      </c>
+      <c r="AH3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>193</v>
+      </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>100</v>
+      </c>
+      <c r="H4">
+        <v>60</v>
+      </c>
+      <c r="I4" t="s">
+        <v>163</v>
+      </c>
+      <c r="J4">
+        <v>0.2</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0.33</v>
+      </c>
+      <c r="N4">
+        <v>-0.33</v>
+      </c>
+      <c r="O4">
+        <v>0.8</v>
+      </c>
+      <c r="P4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Q4">
+        <v>-1</v>
+      </c>
+      <c r="R4">
+        <v>-0.01</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>1.3</v>
+      </c>
+      <c r="U4">
+        <v>0.88</v>
+      </c>
+      <c r="V4">
+        <v>0.9</v>
+      </c>
+      <c r="W4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="X4">
+        <v>1.2</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>59.5</v>
+      </c>
+      <c r="AA4">
+        <v>59.7</v>
+      </c>
+      <c r="AB4">
+        <v>60.3</v>
+      </c>
+      <c r="AC4">
+        <v>60.5</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>0.02</v>
+      </c>
+      <c r="AF4">
+        <v>0.02</v>
+      </c>
+      <c r="AG4">
+        <v>0.1</v>
+      </c>
+      <c r="AH4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>194</v>
+      </c>
+      <c r="E5">
+        <v>8</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>100</v>
+      </c>
+      <c r="H5">
+        <v>60</v>
+      </c>
+      <c r="I5" t="s">
+        <v>163</v>
+      </c>
+      <c r="J5">
+        <v>0.2</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0.33</v>
+      </c>
+      <c r="N5">
+        <v>-0.33</v>
+      </c>
+      <c r="O5">
+        <v>0.8</v>
+      </c>
+      <c r="P5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Q5">
+        <v>-1</v>
+      </c>
+      <c r="R5">
+        <v>-0.01</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>1.3</v>
+      </c>
+      <c r="U5">
+        <v>0.88</v>
+      </c>
+      <c r="V5">
+        <v>0.9</v>
+      </c>
+      <c r="W5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="X5">
+        <v>1.2</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>59.5</v>
+      </c>
+      <c r="AA5">
+        <v>59.7</v>
+      </c>
+      <c r="AB5">
+        <v>60.3</v>
+      </c>
+      <c r="AC5">
+        <v>60.5</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>0.02</v>
+      </c>
+      <c r="AF5">
+        <v>0.02</v>
+      </c>
+      <c r="AG5">
+        <v>0.1</v>
+      </c>
+      <c r="AH5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>195</v>
+      </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>100</v>
+      </c>
+      <c r="H6">
+        <v>60</v>
+      </c>
+      <c r="I6" t="s">
+        <v>163</v>
+      </c>
+      <c r="J6">
+        <v>0.2</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0.33</v>
+      </c>
+      <c r="N6">
+        <v>-0.33</v>
+      </c>
+      <c r="O6">
+        <v>0.8</v>
+      </c>
+      <c r="P6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Q6">
+        <v>-1</v>
+      </c>
+      <c r="R6">
+        <v>-0.01</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>1.3</v>
+      </c>
+      <c r="U6">
+        <v>0.88</v>
+      </c>
+      <c r="V6">
+        <v>0.9</v>
+      </c>
+      <c r="W6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="X6">
+        <v>1.2</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>59.5</v>
+      </c>
+      <c r="AA6">
+        <v>59.7</v>
+      </c>
+      <c r="AB6">
+        <v>60.3</v>
+      </c>
+      <c r="AC6">
+        <v>60.5</v>
+      </c>
+      <c r="AD6">
+        <v>0</v>
+      </c>
+      <c r="AE6">
+        <v>0.02</v>
+      </c>
+      <c r="AF6">
+        <v>0.02</v>
+      </c>
+      <c r="AG6">
+        <v>0.1</v>
+      </c>
+      <c r="AH6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>196</v>
+      </c>
+      <c r="E7">
+        <v>8</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>100</v>
+      </c>
+      <c r="H7">
+        <v>60</v>
+      </c>
+      <c r="I7" t="s">
+        <v>163</v>
+      </c>
+      <c r="J7">
+        <v>0.2</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0.33</v>
+      </c>
+      <c r="N7">
+        <v>-0.33</v>
+      </c>
+      <c r="O7">
+        <v>0.8</v>
+      </c>
+      <c r="P7">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Q7">
+        <v>-1</v>
+      </c>
+      <c r="R7">
+        <v>-0.01</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>1.3</v>
+      </c>
+      <c r="U7">
+        <v>0.88</v>
+      </c>
+      <c r="V7">
+        <v>0.9</v>
+      </c>
+      <c r="W7">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="X7">
+        <v>1.2</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>59.5</v>
+      </c>
+      <c r="AA7">
+        <v>59.7</v>
+      </c>
+      <c r="AB7">
+        <v>60.3</v>
+      </c>
+      <c r="AC7">
+        <v>60.5</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <v>0.02</v>
+      </c>
+      <c r="AF7">
+        <v>0.02</v>
+      </c>
+      <c r="AG7">
+        <v>0.1</v>
+      </c>
+      <c r="AH7">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>197</v>
+      </c>
+      <c r="E8">
+        <v>8</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <v>100</v>
+      </c>
+      <c r="H8">
+        <v>60</v>
+      </c>
+      <c r="I8" t="s">
+        <v>163</v>
+      </c>
+      <c r="J8">
+        <v>0.2</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0.33</v>
+      </c>
+      <c r="N8">
+        <v>-0.33</v>
+      </c>
+      <c r="O8">
+        <v>0.8</v>
+      </c>
+      <c r="P8">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Q8">
+        <v>-1</v>
+      </c>
+      <c r="R8">
+        <v>-0.01</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>1.3</v>
+      </c>
+      <c r="U8">
+        <v>0.88</v>
+      </c>
+      <c r="V8">
+        <v>0.9</v>
+      </c>
+      <c r="W8">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="X8">
+        <v>1.2</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>59.5</v>
+      </c>
+      <c r="AA8">
+        <v>59.7</v>
+      </c>
+      <c r="AB8">
+        <v>60.3</v>
+      </c>
+      <c r="AC8">
+        <v>60.5</v>
+      </c>
+      <c r="AD8">
+        <v>0</v>
+      </c>
+      <c r="AE8">
+        <v>0.02</v>
+      </c>
+      <c r="AF8">
+        <v>0.02</v>
+      </c>
+      <c r="AG8">
+        <v>0.1</v>
+      </c>
+      <c r="AH8">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>198</v>
+      </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9">
+        <v>100</v>
+      </c>
+      <c r="H9">
+        <v>60</v>
+      </c>
+      <c r="I9" t="s">
+        <v>163</v>
+      </c>
+      <c r="J9">
+        <v>0.2</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0.33</v>
+      </c>
+      <c r="N9">
+        <v>-0.33</v>
+      </c>
+      <c r="O9">
+        <v>0.8</v>
+      </c>
+      <c r="P9">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Q9">
+        <v>-1</v>
+      </c>
+      <c r="R9">
+        <v>-0.01</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>1.3</v>
+      </c>
+      <c r="U9">
+        <v>0.88</v>
+      </c>
+      <c r="V9">
+        <v>0.9</v>
+      </c>
+      <c r="W9">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="X9">
+        <v>1.2</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>59.5</v>
+      </c>
+      <c r="AA9">
+        <v>59.7</v>
+      </c>
+      <c r="AB9">
+        <v>60.3</v>
+      </c>
+      <c r="AC9">
+        <v>60.5</v>
+      </c>
+      <c r="AD9">
+        <v>0</v>
+      </c>
+      <c r="AE9">
+        <v>0.02</v>
+      </c>
+      <c r="AF9">
+        <v>0.02</v>
+      </c>
+      <c r="AG9">
+        <v>0.1</v>
+      </c>
+      <c r="AH9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>199</v>
+      </c>
+      <c r="E10">
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <v>100</v>
+      </c>
+      <c r="H10">
+        <v>60</v>
+      </c>
+      <c r="I10" t="s">
+        <v>163</v>
+      </c>
+      <c r="J10">
+        <v>0.2</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0.33</v>
+      </c>
+      <c r="N10">
+        <v>-0.33</v>
+      </c>
+      <c r="O10">
+        <v>0.8</v>
+      </c>
+      <c r="P10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Q10">
+        <v>-1</v>
+      </c>
+      <c r="R10">
+        <v>-0.01</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>1.3</v>
+      </c>
+      <c r="U10">
+        <v>0.88</v>
+      </c>
+      <c r="V10">
+        <v>0.9</v>
+      </c>
+      <c r="W10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="X10">
+        <v>1.2</v>
+      </c>
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>59.5</v>
+      </c>
+      <c r="AA10">
+        <v>59.7</v>
+      </c>
+      <c r="AB10">
+        <v>60.3</v>
+      </c>
+      <c r="AC10">
+        <v>60.5</v>
+      </c>
+      <c r="AD10">
+        <v>0</v>
+      </c>
+      <c r="AE10">
+        <v>0.02</v>
+      </c>
+      <c r="AF10">
+        <v>0.02</v>
+      </c>
+      <c r="AG10">
+        <v>0.1</v>
+      </c>
+      <c r="AH10">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>200</v>
+      </c>
+      <c r="E11">
+        <v>8</v>
+      </c>
+      <c r="F11">
+        <v>5</v>
+      </c>
+      <c r="G11">
+        <v>100</v>
+      </c>
+      <c r="H11">
+        <v>60</v>
+      </c>
+      <c r="I11" t="s">
+        <v>163</v>
+      </c>
+      <c r="J11">
+        <v>0.2</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0.33</v>
+      </c>
+      <c r="N11">
+        <v>-0.33</v>
+      </c>
+      <c r="O11">
+        <v>0.8</v>
+      </c>
+      <c r="P11">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Q11">
+        <v>-1</v>
+      </c>
+      <c r="R11">
+        <v>-0.01</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>1.3</v>
+      </c>
+      <c r="U11">
+        <v>0.88</v>
+      </c>
+      <c r="V11">
+        <v>0.9</v>
+      </c>
+      <c r="W11">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="X11">
+        <v>1.2</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>59.5</v>
+      </c>
+      <c r="AA11">
+        <v>59.7</v>
+      </c>
+      <c r="AB11">
+        <v>60.3</v>
+      </c>
+      <c r="AC11">
+        <v>60.5</v>
+      </c>
+      <c r="AD11">
+        <v>0</v>
+      </c>
+      <c r="AE11">
+        <v>0.02</v>
+      </c>
+      <c r="AF11">
+        <v>0.02</v>
+      </c>
+      <c r="AG11">
+        <v>0.1</v>
+      </c>
+      <c r="AH11">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>